<commit_message>
chore: update ia dataset
</commit_message>
<xml_diff>
--- a/src/lib/ia/event-recommendations/geniusxp-database-next-projects.xlsx
+++ b/src/lib/ia/event-recommendations/geniusxp-database-next-projects.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="221">
   <si>
     <t>nome</t>
   </si>
@@ -130,6 +130,12 @@
     <t>alimentacao;educacao;ia-iot;agronegocio;sustentabilidade</t>
   </si>
   <si>
+    <t>Área da Iniciação Científica</t>
+  </si>
+  <si>
+    <t>14h - 18h</t>
+  </si>
+  <si>
     <t>CyberSecurity CTF</t>
   </si>
   <si>
@@ -145,9 +151,6 @@
     <t>Arena CTF</t>
   </si>
   <si>
-    <t>14h - 18h</t>
-  </si>
-  <si>
     <t>AutoInsight</t>
   </si>
   <si>
@@ -166,6 +169,9 @@
     <t>https://ic-spot-it.vercel.app/</t>
   </si>
   <si>
+    <t>Área da Iniciação Científica (27)</t>
+  </si>
+  <si>
     <t>Pé na Estrada</t>
   </si>
   <si>
@@ -235,6 +241,12 @@
     <t>Ferramenta brasileira de stress testing, a Silentstrike permite analisar aplicações web e realizar diversos testes de estresse. Entre os tipos de ataque suportados estão HTTP Keep Alive, HTTP Slow Post, Post Flood e XML-RPC Flood.</t>
   </si>
   <si>
+    <t>Firewall Arena</t>
+  </si>
+  <si>
+    <t>17h - 18h</t>
+  </si>
+  <si>
     <t>Condelivery</t>
   </si>
   <si>
@@ -307,6 +319,9 @@
     <t>Defesa cibernética</t>
   </si>
   <si>
+    <t>16h - 17h</t>
+  </si>
+  <si>
     <t>DataStorm</t>
   </si>
   <si>
@@ -326,18 +341,6 @@
   </si>
   <si>
     <t>governanca;alimentacao;comercio</t>
-  </si>
-  <si>
-    <t>AutoCare</t>
-  </si>
-  <si>
-    <t>O AutoCare é um serviço desenvolvido para tornar o diagnóstico de problemas veiculares mais fácil, simples e acessível para o usuário comum. Por meio de um chatbot intuitivo, o usuário pode descrever brevemente seu problema e, com o uso de inteligência artificial, o sistema tokeniza essa entrada e a compara com uma base de dados, gerando um diagnóstico provável. Além disso, o AutoCare Bot oferece uma estimativa de custo e a possibilidade de agendar uma consulta com um mecânico parceiro próximo.</t>
-  </si>
-  <si>
-    <t>transporte;seguranca;ia-iot</t>
-  </si>
-  <si>
-    <t>https://autocare-virid.vercel.app/</t>
   </si>
   <si>
     <t>Porção Tropical</t>
@@ -601,12 +604,111 @@
   <si>
     <t>ia-iot</t>
   </si>
+  <si>
+    <t>GAID</t>
+  </si>
+  <si>
+    <t>Solução para auto-diagnósticos, orçamentos, e agendamentos para o ramo automotivo. Uma plataforma de uso recorrente do motorista que o ajuda a manter a saúde do carro, usando de IA e IoT para tornar a vida da pessoa que dirige, mais fácil</t>
+  </si>
+  <si>
+    <t>transporte;ia-iot</t>
+  </si>
+  <si>
+    <t>Gearbox Tracker IA</t>
+  </si>
+  <si>
+    <t>Sistema que utiliza algoritmos de machine learning e análise de vibração para monitorar, em tempo real, o conjunto de embreagem e as engrenagens da caixa de câmbio. O mais interessante é que ele consegue identificar anomalias antes que se tornem problemas graves, garantindo mais segurança e eficiência nas operações. Com criptografia RSA para proteger os dados e uma interface visual intuitiva, a solução tem o potencial de revolucionar o transporte rodoviário com foco em manutenção preditiva.</t>
+  </si>
+  <si>
+    <t>Engenharia Mecatrônica</t>
+  </si>
+  <si>
+    <t>transporte;ia-iot;seguranca</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/posts/gabrielmmagan_inovaaexaetoemmovimento-manutenaexaetopreditiva-activity-7254109706934243329-Z1Gj?utm_source=share&amp;utm_medium=member_desktop</t>
+  </si>
+  <si>
+    <t>RoboBrain</t>
+  </si>
+  <si>
+    <t>O projeto visa desenvolver um robô inteligente capaz de localizar e manipular objetos conforme solicitado pelo usuário. Para alcançar esse objetivo, o robô será equipado com uma câmera integrada para a identificação precisa dos objetos e uma garra para pegá-los com precisão.</t>
+  </si>
+  <si>
+    <t>https://robobrain.vercel.app/</t>
+  </si>
+  <si>
+    <t>InvesteAI</t>
+  </si>
+  <si>
+    <t>Realizamos o rebranding da plataforma FundosNET da B3, que disponibiliza os prospectos de fundos de investimentos, ETFs e outros produtos financeiros. Nosso principal objetivo foi modernizar a experiência do usuário, tornando a plataforma mais acessível e intuitiva. Além disso, integramos um assistente virtual que permite buscas em linguagem natural, facilitando o acesso rápido e preciso às informações desejadas, aprimorando a eficiência na navegação e consulta de dados financeiros.</t>
+  </si>
+  <si>
+    <t>https://investeai.com.br/</t>
+  </si>
+  <si>
+    <t>15h - 16h20</t>
+  </si>
+  <si>
+    <t>Base estelar</t>
+  </si>
+  <si>
+    <t>Base Estelar é um jogo hipercasual desenvolvido em parceria com a Osten Games, criado com o objetivo de oferecer aos usuários uma experiência de jogo acessível, que possa ser aproveitada em qualquer lugar. Com uma mecânica simples e intuitiva, o jogo permite diversão imediata, enquanto também oferece a oportunidade de ganhar recompensas financeiras por meio de um sistema de blockchain integrado, tornando a tecnologia acessível na prática.</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de jogos</t>
+  </si>
+  <si>
+    <t>entretenimento;jogos;banking</t>
+  </si>
+  <si>
+    <t>Totenize</t>
+  </si>
+  <si>
+    <t>A Totenize traz robôs totens interativos que priorizam a acessibilidade, oferecendo suporte à comunicação em Libras, automação de pedidos e pagamentos, e coleta de dados para otimizar a experiência do cliente.</t>
+  </si>
+  <si>
+    <t>StartupOne</t>
+  </si>
+  <si>
+    <t>ia-iot;entretenimento;comunicacao</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1pu6ftd6KBN189fkjAQGaSzglxZDtZ07S/view</t>
+  </si>
+  <si>
+    <t>Drone Arena</t>
+  </si>
+  <si>
+    <t>Arena Drone</t>
+  </si>
+  <si>
+    <t>O projeto foi desenvolvido para solucionar a necessidade de identificar pessoas em situações de risco durante enchentes, como as que ocorreram em abril de 2024 no estado do Rio Grande do Sul. Esse tipo de desastre natural frequentemente resulta em dificuldades para localizar pessoas em áreas inundadas, dificultando operações de resgate e aumentando os riscos para as equipes envolvidas.</t>
+  </si>
+  <si>
+    <t>14h - 15h</t>
+  </si>
+  <si>
+    <t>Sopa de letrinhas</t>
+  </si>
+  <si>
+    <t>Neste jogo multiplayer competitivo, você e mais 14 jogadores competirão para solucionar charadas usando as letras da sopa de letrinhas o mais rápido possível. E lembre-se, o melhor jogador pode ganhar um Echo Dot 5ª geração!</t>
+  </si>
+  <si>
+    <t>LocoMob</t>
+  </si>
+  <si>
+    <t>O LocoMob🚌🚗 é uma solução voltada para Mobilidade como Serviço (MaaS), oferecendo uma aplicação para a gestão inteligente de rotas. Ela permite a criação de rotas personalizadas, com endereços de partida, destino e paradas intermediárias, além de oferecer a opção de seleção entre transporte individual ou coletivo. A plataforma também conta com um sistema de notificações sobre as regras de rodízio no grande centro de São Paulo, alertando os usuários sobre as restrições aplicáveis.</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/posts/gustavoherreronunes_tech-project-future-activity-7255376399660711936-aKOS?utm_source=share&amp;utm_medium=member_desktop</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -630,6 +732,17 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;docs-Calibri&quot;"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <u/>
       <sz val="11.0"/>
       <color rgb="FF0000FF"/>
@@ -643,23 +756,15 @@
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -686,26 +791,23 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -713,20 +815,23 @@
     <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -946,6 +1051,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="25.38"/>
+    <col customWidth="1" min="2" max="2" width="37.75"/>
     <col customWidth="1" min="3" max="3" width="25.13"/>
     <col customWidth="1" min="5" max="6" width="25.5"/>
   </cols>
@@ -993,7 +1099,9 @@
         <v>12</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="2">
+        <v>12.0</v>
+      </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1015,8 +1123,12 @@
         <v>17</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="2">
+        <v>23.0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
@@ -1061,7 +1173,9 @@
       <c r="F5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="2">
+        <v>12.0</v>
+      </c>
       <c r="H5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1107,39 +1221,43 @@
         <v>38</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="G7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>20</v>
@@ -1150,8 +1268,8 @@
       <c r="E9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>47</v>
+      <c r="F9" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="G9" s="2">
         <v>2.0</v>
@@ -1161,11 +1279,11 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
-        <v>48</v>
+      <c r="A10" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
@@ -1177,17 +1295,21 @@
         <v>32</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>20</v>
@@ -1198,8 +1320,8 @@
       <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>53</v>
+      <c r="F11" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="G11" s="2">
         <v>2.0</v>
@@ -1210,13 +1332,13 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>11</v>
@@ -1225,20 +1347,22 @@
         <v>32</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="2">
+        <v>30.0</v>
+      </c>
       <c r="H12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>11</v>
@@ -1256,137 +1380,161 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="G14" s="2">
+        <v>55.0</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="2">
+        <v>24.0</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="G16" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="G17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="G19" s="2">
+        <v>28.0</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>11</v>
@@ -1395,35 +1543,43 @@
         <v>12</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="G20" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="G21" s="2">
+        <v>46.0</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>30</v>
@@ -1432,18 +1588,22 @@
         <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="G22" s="2">
+        <v>36.0</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>16</v>
@@ -1454,60 +1614,72 @@
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="F23" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="2">
+        <v>22.0</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="G24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" s="2">
+        <v>47.0</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>20</v>
@@ -1516,234 +1688,276 @@
         <v>11</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="G26" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" s="2">
+        <v>22.0</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="2">
+        <v>26.0</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" s="9">
+        <v>35.0</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F31" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G32" s="9">
+        <v>35.0</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>30</v>
+        <v>132</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="9">
+        <v>6.0</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G35" s="9">
+        <v>23.0</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="G36" s="7"/>
-      <c r="H36" s="3"/>
+        <v>92</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>20</v>
@@ -1752,18 +1966,22 @@
         <v>11</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
+      <c r="G37" s="2">
+        <v>53.0</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>20</v>
@@ -1772,18 +1990,22 @@
         <v>11</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
+      <c r="G38" s="2">
+        <v>54.0</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>20</v>
@@ -1792,18 +2014,22 @@
         <v>11</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="G39" s="2">
+        <v>53.0</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>20</v>
@@ -1812,170 +2038,188 @@
         <v>11</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="G40" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G41" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G42" s="2">
+        <v>23.0</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G43" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="G44" s="8">
+      <c r="D44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="G44" s="2">
         <v>3.0</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H44" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="C45" s="8" t="s">
+      <c r="A45" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G45" s="8">
+      <c r="D45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="2">
         <v>3.0</v>
       </c>
-      <c r="H45" s="8" t="s">
+      <c r="H45" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>164</v>
+      <c r="A46" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F46" s="10"/>
-      <c r="G46" s="8">
+      <c r="D46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="2">
         <v>3.0</v>
       </c>
-      <c r="H46" s="8" t="s">
-        <v>13</v>
+      <c r="H46" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>166</v>
+      <c r="A47" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="F47" s="10"/>
-      <c r="G47" s="8">
+      <c r="D47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="G47" s="2">
         <v>3.0</v>
       </c>
       <c r="H47" s="12" t="s">
@@ -1983,145 +2227,349 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C48" s="11" t="s">
+      <c r="A48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D48" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="G48" s="8">
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F48" s="13"/>
+      <c r="G48" s="1">
         <v>3.0</v>
       </c>
-      <c r="H48" s="12" t="s">
+      <c r="H48" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F49" s="13"/>
+      <c r="G49" s="1">
+        <v>34.0</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F50" s="13"/>
+      <c r="G50" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="C49" s="13" t="s">
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F51" s="13"/>
+      <c r="G51" s="1">
+        <v>54.0</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1">
+        <v>46.0</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D49" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="F49" s="14"/>
-      <c r="G49" s="13">
-        <v>3.0</v>
-      </c>
-      <c r="H49" s="13" t="s">
+      <c r="D53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F53" s="13"/>
+      <c r="G53" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="C50" s="13" t="s">
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="G54" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="G55" s="2">
+        <v>30.0</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G56" s="2">
+        <v>56.0</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F57" s="13"/>
+      <c r="G57" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F59" s="13"/>
+      <c r="G59" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="13"/>
+      <c r="G60" s="2">
+        <v>22.0</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D50" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F50" s="14"/>
-      <c r="G50" s="13">
-        <v>34.0</v>
-      </c>
-      <c r="H50" s="13" t="s">
+      <c r="D61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="G61" s="1">
+        <v>35.0</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="F52" s="14"/>
-      <c r="G52" s="13">
-        <v>54.0</v>
-      </c>
-      <c r="H52" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13">
-        <v>46.0</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2138,16 +2586,20 @@
     <hyperlink r:id="rId10" ref="F28"/>
     <hyperlink r:id="rId11" ref="F29"/>
     <hyperlink r:id="rId12" ref="F30"/>
-    <hyperlink r:id="rId13" ref="F31"/>
-    <hyperlink r:id="rId14" ref="F33"/>
+    <hyperlink r:id="rId13" ref="F32"/>
+    <hyperlink r:id="rId14" ref="F34"/>
     <hyperlink r:id="rId15" ref="F35"/>
-    <hyperlink r:id="rId16" ref="F36"/>
+    <hyperlink r:id="rId16" ref="F41"/>
     <hyperlink r:id="rId17" ref="F42"/>
     <hyperlink r:id="rId18" ref="F43"/>
     <hyperlink r:id="rId19" ref="F44"/>
-    <hyperlink r:id="rId20" ref="F45"/>
-    <hyperlink r:id="rId21" ref="F48"/>
+    <hyperlink r:id="rId20" ref="F47"/>
+    <hyperlink r:id="rId21" ref="F54"/>
+    <hyperlink r:id="rId22" ref="F55"/>
+    <hyperlink r:id="rId23" ref="F56"/>
+    <hyperlink r:id="rId24" ref="F58"/>
+    <hyperlink r:id="rId25" ref="F61"/>
   </hyperlinks>
-  <drawing r:id="rId22"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>